<commit_message>
Initial commit - Real-Time OCR Project
</commit_message>
<xml_diff>
--- a/ocr_results.xlsx
+++ b/ocr_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,445 +451,713 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>FramesUsed</t>
+          <t>Vote Count</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sundaram-Clayicn [ Lim</t>
+          <t>8B</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>70.93000000000001</v>
+        <v>99</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-10-28 14:22:39</t>
+          <t>2025-10-31 15:06:06</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>#rd</t>
+          <t>88</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6.65</v>
+        <v>96.40000000000001</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-10-28 14:28:36</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
+          <t>2025-10-31 15:06:12</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>8rtr 48o</t>
+          <t>8B</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7.48</v>
+        <v>94.59999999999999</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-10-28 14:28:38</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
+          <t>2025-10-31 15:06:14</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Pide</t>
+          <t>RI-K</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>11.22</v>
+        <v>48.8</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-10-28 14:28:39</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
+          <t>2025-10-31 15:06:50</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>8B</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7.24</v>
+        <v>39</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-10-28 14:28:39</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
+          <t>2025-10-31 15:07:32</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>y</t>
+          <t>RO-K</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>75.98</v>
+        <v>69.90000000000001</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-10-28 14:28:41</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
+          <t>2025-10-31 15:07:41</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Sundaram-Clayton Limited ,</t>
+          <t>RI-K</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>91.63</v>
+        <v>88.09999999999999</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-10-28 14:33:00</t>
+          <t>2025-10-31 15:08:43</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>W Andtin-trmnL</t>
+          <t>8B</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>42.15</v>
+        <v>89.3</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-10-28 14:37:34</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
+          <t>2025-10-31 15:10:25</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>QT Bef baie . a ‘ie Rape SS Aee</t>
+          <t>RO-K</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>15.22</v>
+        <v>36.4</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-10-28 15:27:01</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
+          <t>2025-10-31 15:10:49</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>LS ar NE ae ge</t>
+          <t>RI-K</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>27.2</v>
+        <v>40.9</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-10-28 15:27:04</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
+          <t>2025-10-31 15:11:03</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>o ee ey ie ta Lila ES Wow .</t>
+          <t>8B</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>27.89</v>
+        <v>40.4</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-10-28 15:27:07</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
+          <t>2025-10-31 16:29:33</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Vo tie 7 Eo ag _fa eae Aes | ..</t>
+          <t>RI-K</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>30.5</v>
+        <v>88.8</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-10-28 15:27:11</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
+          <t>2025-10-31 16:31:42</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>fee ee</t>
+          <t>RI-K</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>22.5</v>
+        <v>58.1</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-10-28 15:27:14</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
+          <t>2025-10-31 16:32:02</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ge hf tf eles ad ane J Re aj ayer: :) ey _tg. Die’ Ses.</t>
+          <t>8B</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>26.93</v>
+        <v>93.8</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-10-28 15:27:17</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
+          <t>2025-10-31 16:32:10</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>eps k SE See cote p es SESE ere tie wen a Hehe Pad Nett bad Sai tetas 2ST per he tibeeicng SEES sire Ae ere Serna Sait ae ss ceivigth eal ad Ba AS pte rat got ep ite ep ola Aare ee dae br af ayied le PE yh eh tns eo ara Daas ety ge ye eS eT any oe perp RL eo Ret int Sor Re gt age al Pesca he ae re ey ye aah Bd ee A A ete COE Le Et ont ot qi eer asst ie eo Pe ee) Pe spain kent ite eam ee os gee ant A crear qe yet ree) TO cee sah Fee as EARLS Gio ig as WEEN er le ee ee ee</t>
+          <t>8B</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>16.43</v>
+        <v>86.40000000000001</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-10-28 15:27:24</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr"/>
+          <t>2025-11-01 09:15:45</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>© amiengl ey iB</t>
+          <t>RI-K</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>25.75</v>
+        <v>76.5</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-10-28 15:27:27</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr"/>
+          <t>2025-11-01 09:18:01</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Sundaram-Clyicn Lintr]</t>
+          <t>85</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>44.79</v>
+        <v>41.7</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-10-28 15:28:10</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr"/>
+          <t>2025-11-01 09:18:30</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Sundaram-Claylon Limticd</t>
+          <t>8B</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>63.06</v>
+        <v>96.90000000000001</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-10-28 15:28:13</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr"/>
+          <t>2025-11-01 09:18:40</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Sundaram-Clayton Limicd</t>
+          <t>8E</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>67.76000000000001</v>
+        <v>-1</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-10-28 15:28:16</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr"/>
+          <t>2025-11-01 10:08:02</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Sundarar-Clayton Limted</t>
+          <t>8B</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>79.27</v>
+        <v>99.8</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-10-28 15:28:19</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr"/>
+          <t>2025-11-01 10:08:06</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Sundaram-Clayton Limite</t>
+          <t>RI-K</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>99.14</v>
+        <v>93.90000000000001</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-10-28 15:30:23</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr"/>
+          <t>2025-11-01 10:08:22</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Sundaram-Clayton Limit</t>
+          <t>RA-K</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>97.22</v>
+        <v>20.8</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-10-28 15:30:26</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr"/>
+          <t>2025-11-01 10:14:30</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Sundaram-Clayton Limited</t>
+          <t>RO-K</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>92.03</v>
+        <v>23.1</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-10-28 15:30:29</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr"/>
+          <t>2025-11-01 10:14:35</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>undaram-Clayton Limite</t>
+          <t>RA-K</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>99.19</v>
+        <v>43.7</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-10-28 16:04:55</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr"/>
+          <t>2025-11-01 10:14:43</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Sundaram-Clayton Lim</t>
+          <t>8B</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>98.34999999999999</v>
+        <v>95.8</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-10-28 16:04:58</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr"/>
+          <t>2025-11-01 10:15:24</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Limited Isundaram-Clayton</t>
+          <t>RI-K</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>93.75</v>
+        <v>39.4</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-10-28 16:05:01</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr"/>
+          <t>2025-11-01 10:15:45</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Sundaram-Clayton Limited</t>
+          <t>TS</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>99.91</v>
+        <v>42</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-10-28 16:05:05</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr"/>
+          <t>2025-11-01 10:16:40</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>SS</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>59</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2025-11-01 10:17:03</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>36.1</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2025-11-01 10:17:24</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>8B</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>97.5</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2025-11-01 10:17:32</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>8B</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>97.3</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2025-11-01 10:18:42</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>RI-K</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>84.8</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2025-11-01 10:19:00</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>RA-K</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>72.7</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2025-11-01 11:04:19</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>RO-K</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>41.1</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2025-11-01 11:04:37</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>RA-K</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>85</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2025-11-01 11:04:38</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>RI-K</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>91.3</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2025-11-01 11:04:46</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>8B</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>93.40000000000001</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2025-11-01 11:05:12</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>8B</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>99.3</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2025-11-01 11:46:36</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>RI-K</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>88.0</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2025-11-01 11:46:46</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>